<commit_message>
Actualizacion capabilities and base_test
</commit_message>
<xml_diff>
--- a/AutomationFramework/excel_logs/hardware_test_hw_component_logs.xlsx
+++ b/AutomationFramework/excel_logs/hardware_test_hw_component_logs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,6 +473,210 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This test is to get description components.
+</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>&lt;class 'AutomationFramework.page_objects.hardware.hardware.Hardware'&gt;</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>hw_component_description</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>&lt;get&gt;
+  &lt;filter&gt;
+    &lt;components xmlns="http://openconfig.net/yang/platform"&gt;
+      &lt;component&gt;
+        &lt;name&gt;CHASIS&lt;/name&gt;
+        &lt;state&gt;
+          &lt;description&gt;&lt;/description&gt;
+        &lt;/state&gt;
+      &lt;/component&gt;
+    &lt;/components&gt;
+  &lt;/filter&gt;
+&lt;/get&gt;</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;
+&lt;rpc-reply message-id="urn:uuid:a9db80e4-4328-4d02-8edf-2b21b768cab6"
+ xmlns:ncx="http://netconfcentral.org/ns/yuma-ncx"
+ ncx:last-modified="2020-10-07T13:51:28Z" ncx:etag="814"
+ xmlns="urn:ietf:params:xml:ns:netconf:base:1.0"&gt;
+ &lt;data&gt;&lt;/data&gt;
+&lt;/rpc-reply&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This test is to get the hardware version components.
+</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>&lt;class 'AutomationFramework.page_objects.hardware.hardware.Hardware'&gt;</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>hw_component_hardware_version</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>&lt;get&gt;
+  &lt;filter&gt;
+    &lt;components xmlns="http://openconfig.net/yang/platform"&gt;
+      &lt;component&gt;
+        &lt;name&gt;CHASIS&lt;/name&gt;
+        &lt;state&gt;
+          &lt;hardware-version&gt;&lt;/hardware-version&gt;
+        &lt;/state&gt;
+      &lt;/component&gt;
+    &lt;/components&gt;
+  &lt;/filter&gt;
+&lt;/get&gt;</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;
+&lt;rpc-reply message-id="urn:uuid:770b8d52-6123-4d3f-9c3b-94a954bd3ed3"
+ xmlns:ncx="http://netconfcentral.org/ns/yuma-ncx"
+ ncx:last-modified="2020-10-07T13:51:28Z" ncx:etag="814"
+ xmlns="urn:ietf:params:xml:ns:netconf:base:1.0"&gt;
+ &lt;data&gt;&lt;/data&gt;
+&lt;/rpc-reply&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This test is to get the component id.
+</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>&lt;class 'AutomationFramework.page_objects.hardware.hardware.Hardware'&gt;</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>hw_component_id</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>&lt;get&gt;
+  &lt;filter&gt;
+    &lt;components xmlns="http://openconfig.net/yang/platform"&gt;
+      &lt;component&gt;
+        &lt;name&gt;CHASIS&lt;/name&gt;
+        &lt;state&gt;
+          &lt;id&gt;&lt;/id&gt;
+        &lt;/state&gt;
+      &lt;/component&gt;
+    &lt;/components&gt;
+  &lt;/filter&gt;
+&lt;/get&gt;</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;
+&lt;rpc-reply message-id="urn:uuid:e182e267-14e7-4605-924e-8b7fc69051a4"
+ xmlns:ncx="http://netconfcentral.org/ns/yuma-ncx"
+ ncx:last-modified="2020-10-07T13:51:28Z" ncx:etag="814"
+ xmlns="urn:ietf:params:xml:ns:netconf:base:1.0"&gt;
+ &lt;data&gt;&lt;/data&gt;
+&lt;/rpc-reply&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This test is to get location components.
+</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>&lt;class 'AutomationFramework.page_objects.hardware.hardware.Hardware'&gt;</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>hw_component_location</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>&lt;get&gt;
+  &lt;filter&gt;
+    &lt;components xmlns="http://openconfig.net/yang/platform"&gt;
+      &lt;component&gt;
+        &lt;name&gt;CHASIS&lt;/name&gt;
+        &lt;state&gt;
+          &lt;location&gt;&lt;/location&gt;
+        &lt;/state&gt;
+      &lt;/component&gt;
+    &lt;/components&gt;
+  &lt;/filter&gt;
+&lt;/get&gt;</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;
+&lt;rpc-reply message-id="urn:uuid:ced8c9f7-efd4-46a8-b0a2-e4fab569c00c"
+ xmlns:ncx="http://netconfcentral.org/ns/yuma-ncx"
+ ncx:last-modified="2020-10-07T13:51:28Z" ncx:etag="814"
+ xmlns="urn:ietf:params:xml:ns:netconf:base:1.0"&gt;
+ &lt;data&gt;&lt;/data&gt;
+&lt;/rpc-reply&gt;</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualizacion tests hw component
</commit_message>
<xml_diff>
--- a/AutomationFramework/excel_logs/hardware_test_hw_component_logs.xlsx
+++ b/AutomationFramework/excel_logs/hardware_test_hw_component_logs.xlsx
@@ -501,7 +501,7 @@
   &lt;filter&gt;
     &lt;components xmlns="http://openconfig.net/yang/platform"&gt;
       &lt;component&gt;
-        &lt;name&gt;CHASIS&lt;/name&gt;
+        &lt;name&gt;Waveserver-Ai&lt;/name&gt;
         &lt;state&gt;
           &lt;description&gt;&lt;/description&gt;
         &lt;/state&gt;
@@ -514,11 +514,20 @@
       <c r="J2" t="inlineStr">
         <is>
           <t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;
-&lt;rpc-reply message-id="urn:uuid:a9db80e4-4328-4d02-8edf-2b21b768cab6"
+&lt;rpc-reply message-id="urn:uuid:1924bced-b91c-472c-8c3c-30d51b7bef9e"
  xmlns:ncx="http://netconfcentral.org/ns/yuma-ncx"
  ncx:last-modified="2020-10-07T13:51:28Z" ncx:etag="814"
  xmlns="urn:ietf:params:xml:ns:netconf:base:1.0"&gt;
- &lt;data&gt;&lt;/data&gt;
+ &lt;data&gt;
+  &lt;components xmlns="http://openconfig.net/yang/platform"&gt;
+   &lt;component&gt;
+    &lt;name&gt;Waveserver-Ai&lt;/name&gt;
+    &lt;state&gt;
+     &lt;description&gt;Waveserver Ai Chassis 3-slot, 1RU&lt;/description&gt;
+    &lt;/state&gt;
+   &lt;/component&gt;
+  &lt;/components&gt;
+ &lt;/data&gt;
 &lt;/rpc-reply&gt;</t>
         </is>
       </c>
@@ -551,7 +560,7 @@
   &lt;filter&gt;
     &lt;components xmlns="http://openconfig.net/yang/platform"&gt;
       &lt;component&gt;
-        &lt;name&gt;CHASIS&lt;/name&gt;
+        &lt;name&gt;Waveserver-Ai&lt;/name&gt;
         &lt;state&gt;
           &lt;hardware-version&gt;&lt;/hardware-version&gt;
         &lt;/state&gt;
@@ -564,11 +573,20 @@
       <c r="J3" t="inlineStr">
         <is>
           <t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;
-&lt;rpc-reply message-id="urn:uuid:770b8d52-6123-4d3f-9c3b-94a954bd3ed3"
+&lt;rpc-reply message-id="urn:uuid:f6bb4233-a6c3-495a-8e64-331b2883593a"
  xmlns:ncx="http://netconfcentral.org/ns/yuma-ncx"
  ncx:last-modified="2020-10-07T13:51:28Z" ncx:etag="814"
  xmlns="urn:ietf:params:xml:ns:netconf:base:1.0"&gt;
- &lt;data&gt;&lt;/data&gt;
+ &lt;data&gt;
+  &lt;components xmlns="http://openconfig.net/yang/platform"&gt;
+   &lt;component&gt;
+    &lt;name&gt;Waveserver-Ai&lt;/name&gt;
+    &lt;state&gt;
+     &lt;hardware-version&gt;001&lt;/hardware-version&gt;
+    &lt;/state&gt;
+   &lt;/component&gt;
+  &lt;/components&gt;
+ &lt;/data&gt;
 &lt;/rpc-reply&gt;</t>
         </is>
       </c>
@@ -601,7 +619,7 @@
   &lt;filter&gt;
     &lt;components xmlns="http://openconfig.net/yang/platform"&gt;
       &lt;component&gt;
-        &lt;name&gt;CHASIS&lt;/name&gt;
+        &lt;name&gt;Waveserver-Ai&lt;/name&gt;
         &lt;state&gt;
           &lt;id&gt;&lt;/id&gt;
         &lt;/state&gt;
@@ -614,11 +632,20 @@
       <c r="J4" t="inlineStr">
         <is>
           <t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;
-&lt;rpc-reply message-id="urn:uuid:e182e267-14e7-4605-924e-8b7fc69051a4"
+&lt;rpc-reply message-id="urn:uuid:aa1f2b73-992f-4608-8b3a-2c44ceafe004"
  xmlns:ncx="http://netconfcentral.org/ns/yuma-ncx"
  ncx:last-modified="2020-10-07T13:51:28Z" ncx:etag="814"
  xmlns="urn:ietf:params:xml:ns:netconf:base:1.0"&gt;
- &lt;data&gt;&lt;/data&gt;
+ &lt;data&gt;
+  &lt;components xmlns="http://openconfig.net/yang/platform"&gt;
+   &lt;component&gt;
+    &lt;name&gt;Waveserver-Ai&lt;/name&gt;
+    &lt;state&gt;
+     &lt;id&gt;Waveserver Ai Chassis&lt;/id&gt;
+    &lt;/state&gt;
+   &lt;/component&gt;
+  &lt;/components&gt;
+ &lt;/data&gt;
 &lt;/rpc-reply&gt;</t>
         </is>
       </c>
@@ -653,7 +680,7 @@
   &lt;filter&gt;
     &lt;components xmlns="http://openconfig.net/yang/platform"&gt;
       &lt;component&gt;
-        &lt;name&gt;CHASIS&lt;/name&gt;
+        &lt;name&gt;Waveserver-Ai&lt;/name&gt;
         &lt;state&gt;
           &lt;location&gt;&lt;/location&gt;
         &lt;/state&gt;
@@ -668,11 +695,19 @@
       <c r="J5" t="inlineStr">
         <is>
           <t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;
-&lt;rpc-reply message-id="urn:uuid:ced8c9f7-efd4-46a8-b0a2-e4fab569c00c"
+&lt;rpc-reply message-id="urn:uuid:393b75be-0861-4ec9-b887-37269807287d"
  xmlns:ncx="http://netconfcentral.org/ns/yuma-ncx"
  ncx:last-modified="2020-10-07T13:51:28Z" ncx:etag="814"
  xmlns="urn:ietf:params:xml:ns:netconf:base:1.0"&gt;
- &lt;data&gt;&lt;/data&gt;
+ &lt;data&gt;
+  &lt;components xmlns="http://openconfig.net/yang/platform"&gt;
+   &lt;component&gt;
+    &lt;name&gt;Waveserver-Ai&lt;/name&gt;
+    &lt;state&gt;
+    &lt;/state&gt;
+   &lt;/component&gt;
+  &lt;/components&gt;
+ &lt;/data&gt;
 &lt;/rpc-reply&gt;</t>
         </is>
       </c>

</xml_diff>

<commit_message>
Añadido tests hw component_psu_transceiver y fan
</commit_message>
<xml_diff>
--- a/AutomationFramework/excel_logs/hardware_test_hw_component_logs.xlsx
+++ b/AutomationFramework/excel_logs/hardware_test_hw_component_logs.xlsx
@@ -514,7 +514,7 @@
       <c r="J2" t="inlineStr">
         <is>
           <t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;
-&lt;rpc-reply message-id="urn:uuid:e97bf60f-3e4b-4d13-9bb8-52a57e15824e"
+&lt;rpc-reply message-id="urn:uuid:7dc29a4a-195a-4e3a-b5fd-9d3528afee08"
  xmlns:ncx="http://netconfcentral.org/ns/yuma-ncx"
  ncx:last-modified="2020-10-07T13:51:28Z" ncx:etag="814"
  xmlns="urn:ietf:params:xml:ns:netconf:base:1.0"&gt;
@@ -573,7 +573,7 @@
       <c r="J3" t="inlineStr">
         <is>
           <t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;
-&lt;rpc-reply message-id="urn:uuid:46ab6473-6fbe-44da-be2e-1a95719f1517"
+&lt;rpc-reply message-id="urn:uuid:3c13dc21-94ad-4cf0-a2b9-4da9dc00efcd"
  xmlns:ncx="http://netconfcentral.org/ns/yuma-ncx"
  ncx:last-modified="2020-10-07T13:51:28Z" ncx:etag="814"
  xmlns="urn:ietf:params:xml:ns:netconf:base:1.0"&gt;
@@ -632,7 +632,7 @@
       <c r="J4" t="inlineStr">
         <is>
           <t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;
-&lt;rpc-reply message-id="urn:uuid:65ca91d0-06b5-4aa4-b2e8-8d8184255e65"
+&lt;rpc-reply message-id="urn:uuid:bb320285-691f-4e73-a08b-5ab5727f8a58"
  xmlns:ncx="http://netconfcentral.org/ns/yuma-ncx"
  ncx:last-modified="2020-10-07T13:51:28Z" ncx:etag="814"
  xmlns="urn:ietf:params:xml:ns:netconf:base:1.0"&gt;
@@ -695,7 +695,7 @@
       <c r="J5" t="inlineStr">
         <is>
           <t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;
-&lt;rpc-reply message-id="urn:uuid:b11e67a3-bddb-42b5-bcc1-1e9d4ebb6ed2"
+&lt;rpc-reply message-id="urn:uuid:bf787d04-6c1c-41b1-84cf-88218c3f3119"
  xmlns:ncx="http://netconfcentral.org/ns/yuma-ncx"
  ncx:last-modified="2020-10-07T13:51:28Z" ncx:etag="814"
  xmlns="urn:ietf:params:xml:ns:netconf:base:1.0"&gt;

</xml_diff>